<commit_message>
new ui actions - import and clean
</commit_message>
<xml_diff>
--- a/test-input/suite-1/add-steps-in-new-test.xlsx
+++ b/test-input/suite-1/add-steps-in-new-test.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\java\git-repos\poc-tam\server\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\tool-tests\test-input\suite-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDCB8035-787B-476C-85A6-3ACE73C449B9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1815" yWindow="-15870" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1815" yWindow="-15870" windowWidth="25440" windowHeight="15390"/>
   </bookViews>
   <sheets>
     <sheet name="Case" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="30">
   <si>
     <t>Test Object</t>
   </si>
@@ -92,12 +91,30 @@
   </si>
   <si>
     <t>object=Tool;name=tool;action=toCasesTab</t>
+  </si>
+  <si>
+    <t>object=CasesTab;name=casesTab;action=addSuite;arguments=suiteName:suite-1</t>
+  </si>
+  <si>
+    <t>object=CasesTab;name=casesTab;action=openSuite;arguments=suiteName:suite-1</t>
+  </si>
+  <si>
+    <t>object=Suite;name=suite-1;action=addTest;arguments=testName:test-1</t>
+  </si>
+  <si>
+    <t>object=Suite;name=suite-1;action=openTest;arguments=testName:test-1</t>
+  </si>
+  <si>
+    <t>object=Test;name=test-1;action=hasTotalSteps;arguments=numberOfSteps:0</t>
+  </si>
+  <si>
+    <t>object=Test;name=test-1;action=addStep;arguments=object:Tool, name:tool, action:toCasesTab</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -442,14 +459,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="88.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -463,7 +485,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -477,7 +499,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -491,7 +513,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -505,7 +527,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -519,7 +541,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -533,7 +555,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -547,7 +569,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -559,6 +581,90 @@
       </c>
       <c r="D8" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
revert arguments parsing changes
</commit_message>
<xml_diff>
--- a/test-input/suite-1/add-steps-in-new-test.xlsx
+++ b/test-input/suite-1/add-steps-in-new-test.xlsx
@@ -126,16 +126,16 @@
     <t>row=5;arguments={testName:test-1}</t>
   </si>
   <si>
-    <t>object=Test;name=test-1;action=hasTotalSteps;arguments={numberOfSteps:0}</t>
-  </si>
-  <si>
-    <t>row=6;arguments={numberOfSteps:0}</t>
-  </si>
-  <si>
     <t>object=Test;name=test-1;action=addStep;arguments={object:Tool, name:tool, action:toCasesTab}</t>
   </si>
   <si>
     <t>row=7;arguments={object:Tool, name:tool, action:toCasesTab}</t>
+  </si>
+  <si>
+    <t>object=Test;name=test-1;action=hasTotalSteps;arguments={numberOfSteps:'0'}</t>
+  </si>
+  <si>
+    <t>row=6;arguments={numberOfSteps:'0'}</t>
   </si>
 </sst>
 </file>
@@ -496,8 +496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -798,7 +798,7 @@
         <v>18</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -812,7 +812,7 @@
         <v>22</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -826,7 +826,7 @@
         <v>18</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -840,7 +840,7 @@
         <v>22</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tests for name input
</commit_message>
<xml_diff>
--- a/test-input/suite-1/add-steps-in-new-test.xlsx
+++ b/test-input/suite-1/add-steps-in-new-test.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="52">
   <si>
     <t>Tool</t>
   </si>
@@ -78,9 +78,6 @@
     <t>addStep</t>
   </si>
   <si>
-    <t>object=Tool;name=tool;action=toCasesTab</t>
-  </si>
-  <si>
     <t>importData</t>
   </si>
   <si>
@@ -105,37 +102,79 @@
     <t>object=CasesTab;name=casesTab;action=addSuite;arguments={suiteName:suite-1}</t>
   </si>
   <si>
+    <t>object=CasesTab;name=casesTab;action=openSuite;arguments={suiteName:suite-1}</t>
+  </si>
+  <si>
+    <t>row=3;arguments={suiteName:suite-1}</t>
+  </si>
+  <si>
+    <t>object=Suite;name=suite-1;action=addTest;arguments={testName:test-1}</t>
+  </si>
+  <si>
+    <t>object=Suite;name=suite-1;action=openTest;arguments={testName:test-1}</t>
+  </si>
+  <si>
+    <t>row=5;arguments={testName:test-1}</t>
+  </si>
+  <si>
+    <t>object=Test;name=test-1;action=addStep;arguments={object:Tool, name:tool, action:toCasesTab}</t>
+  </si>
+  <si>
+    <t>object=Test;name=test-1;action=hasTotalSteps;arguments={numberOfSteps:'0'}</t>
+  </si>
+  <si>
+    <t>AddStepForm</t>
+  </si>
+  <si>
+    <t>form</t>
+  </si>
+  <si>
+    <t>selectObject</t>
+  </si>
+  <si>
+    <t>object=Tool</t>
+  </si>
+  <si>
+    <t>hasLocationNames</t>
+  </si>
+  <si>
+    <t>names=[tool]</t>
+  </si>
+  <si>
+    <t>hasNamesStartWith</t>
+  </si>
+  <si>
+    <t>name=too;suggestions=[tool]</t>
+  </si>
+  <si>
+    <t>addAndSelectNewName</t>
+  </si>
+  <si>
+    <t>name=tool</t>
+  </si>
+  <si>
+    <t>selectAction</t>
+  </si>
+  <si>
+    <t>action=toCasesTab</t>
+  </si>
+  <si>
+    <t>clickAddStep</t>
+  </si>
+  <si>
+    <t>numberOfSteps=1</t>
+  </si>
+  <si>
     <t>row=2;arguments={suiteName:suite-1}</t>
   </si>
   <si>
-    <t>object=CasesTab;name=casesTab;action=openSuite;arguments={suiteName:suite-1}</t>
-  </si>
-  <si>
-    <t>row=3;arguments={suiteName:suite-1}</t>
-  </si>
-  <si>
-    <t>object=Suite;name=suite-1;action=addTest;arguments={testName:test-1}</t>
-  </si>
-  <si>
     <t>row=4;arguments={testName:test-1}</t>
   </si>
   <si>
-    <t>object=Suite;name=suite-1;action=openTest;arguments={testName:test-1}</t>
-  </si>
-  <si>
-    <t>row=5;arguments={testName:test-1}</t>
-  </si>
-  <si>
-    <t>object=Test;name=test-1;action=addStep;arguments={object:Tool, name:tool, action:toCasesTab}</t>
+    <t>row=6;arguments={numberOfSteps:'0'}</t>
   </si>
   <si>
     <t>row=7;arguments={object:Tool, name:tool, action:toCasesTab}</t>
-  </si>
-  <si>
-    <t>object=Test;name=test-1;action=hasTotalSteps;arguments={numberOfSteps:'0'}</t>
-  </si>
-  <si>
-    <t>row=6;arguments={numberOfSteps:'0'}</t>
   </si>
 </sst>
 </file>
@@ -494,10 +533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,16 +548,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -529,10 +568,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
         <v>20</v>
-      </c>
-      <c r="D2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -663,86 +702,86 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="D12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="C13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="D13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>28</v>
+        <v>40</v>
+      </c>
+      <c r="D14" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="C15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>29</v>
+        <v>42</v>
+      </c>
+      <c r="D15" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="C16" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>30</v>
+        <v>44</v>
+      </c>
+      <c r="D16" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="C17" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>31</v>
+        <v>46</v>
+      </c>
+      <c r="D17" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -753,41 +792,41 @@
         <v>15</v>
       </c>
       <c r="C18" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>32</v>
+        <v>16</v>
+      </c>
+      <c r="D18" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="B19" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="C19" t="s">
-        <v>18</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
+      </c>
+      <c r="D19" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="B20" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="C20" t="s">
-        <v>22</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="D20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>14</v>
       </c>
@@ -798,10 +837,10 @@
         <v>18</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>14</v>
       </c>
@@ -809,10 +848,10 @@
         <v>15</v>
       </c>
       <c r="C22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -826,7 +865,7 @@
         <v>18</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -837,10 +876,122 @@
         <v>15</v>
       </c>
       <c r="C24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" t="s">
+        <v>21</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" t="s">
+        <v>21</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29" t="s">
+        <v>15</v>
+      </c>
+      <c r="C29" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>14</v>
+      </c>
+      <c r="B30" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>14</v>
+      </c>
+      <c r="B31" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>14</v>
+      </c>
+      <c r="B32" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32" t="s">
+        <v>21</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>